<commit_message>
change function spilt_system, spilt_int_mapp
</commit_message>
<xml_diff>
--- a/output/2023-03-03/gen_parameter_20230303.xlsx
+++ b/output/2023-03-03/gen_parameter_20230303.xlsx
@@ -7,7 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="int_mapping" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="system_name" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="add_suffix_system_name" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +416,25 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A22"/>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,84 +445,248 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>- LIST_INT_MAPPING</t>
+          <t>MVP1</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>['INT_E_LQ_GL_ACCT_SEGMENT_D','INT_E_LQ_GL_BAL_SUM_OC_D','INT_E_LQ_GL_BAL_SUM_RC_D','INT_E_LQ_GL_OC_SEGMENT_D','INT_E_LQ_GL_PROD_SEGMENT_D','INT_E_LQ_GL_RC_SEGMENT_D','INT_E_LQ_IM_ST_DAILY_D','INT_E_LQ_LN_BR_FOREIGN_MKT_D','INT_L_BI_EDW_PARAM_ATS_COMP_CD','INT_L_CCP_EDW_TXNALSB2K','INT_L_EPP_EDW_RPTDDET','INT_L_EPP_EDW_RPTDDET_T1','INT_L_IM_FC_IMBCRM_1_0','INT_L_IM_IMACTM_A_0','INT_L_RBF_EDW_SDL_CLEANSING','INT_L_RCR_EVENTCODE','INT_L_WLS_EDW_WLSPARAM','INT_L_WLS_EDW_WLSPROD','INT_T_CCP_TXNALSB2K_01','INT_T_RCR_EVENTCODE_01','INT_T_WLS_WLSPROD_01']</t>
+          <t>['INT_L_EPP_EDW_RPTDDET','INT_L_EPP_EDW_RPTDDET_T1','INT_L_IM_FC_IMBCRM_1_0','INT_L_IM_IMACTM_A_0']</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>MVP2</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>- LIST_SYSTEM_NAME</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>ACTM,AM,AML,ATM,BCC,BCM,BI,BIFI,CB,CCB,CCP,CDD,CFO,CHYO,CIM,CSENT,CSM,CVA,EDW,EFS,ENL,ESL,ESN,FES,GN,INV,IPS,LCS,LEAD_UL,LQ,MMS,MRP,MUREX,OBM,OLS,PDPA,PLPS,PMH,PRM,RBF,RCR,RDS,SBG,TMS,TRD,WLS,WSS,SCBL</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>- LIST_FULL_SYSTEM_NAME</t>
+          <t>['INT_E_LQ_GL_ACCT_SEGMENT_D','INT_E_LQ_GL_BAL_SUM_OC_D','INT_E_LQ_GL_BAL_SUM_RC_D','INT_E_LQ_GL_OC_SEGMENT_D','INT_E_LQ_GL_PROD_SEGMENT_D','INT_E_LQ_GL_RC_SEGMENT_D','INT_E_LQ_IM_ST_DAILY_D','INT_E_LQ_LN_BR_FOREIGN_MKT_D','INT_L_CCP_EDW_TXNALSB2K','INT_T_CCP_TXNALSB2K_01','INT_L_RCR_EVENTCODE','INT_T_RCR_EVENTCODE_01','INT_L_WLS_EDW_WLSPARAM','INT_L_WLS_EDW_WLSPROD','INT_T_WLS_WLSPROD_01']</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MVP3</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>['INT_L_RBF_EDW_SDL_CLEANSING']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>['REGISTER_CONFIG_SYSTEM_ACTM','REGISTER_CONFIG_SYSTEM_AM','REGISTER_CONFIG_SYSTEM_AML','REGISTER_CONFIG_SYSTEM_ATM','REGISTER_CONFIG_SYSTEM_BCC','REGISTER_CONFIG_SYSTEM_BCM','REGISTER_CONFIG_SYSTEM_BI','REGISTER_CONFIG_SYSTEM_BIFI','REGISTER_CONFIG_SYSTEM_CB','REGISTER_CONFIG_SYSTEM_CCB','REGISTER_CONFIG_SYSTEM_CCP','REGISTER_CONFIG_SYSTEM_CDD','REGISTER_CONFIG_SYSTEM_CFO','REGISTER_CONFIG_SYSTEM_CHYO','REGISTER_CONFIG_SYSTEM_CIM','REGISTER_CONFIG_SYSTEM_CSENT','REGISTER_CONFIG_SYSTEM_CSM','REGISTER_CONFIG_SYSTEM_CVA','REGISTER_CONFIG_SYSTEM_EDW','REGISTER_CONFIG_SYSTEM_EFS','REGISTER_CONFIG_SYSTEM_ENL','REGISTER_CONFIG_SYSTEM_ESL','REGISTER_CONFIG_SYSTEM_ESN','REGISTER_CONFIG_SYSTEM_FES','REGISTER_CONFIG_SYSTEM_GN','REGISTER_CONFIG_SYSTEM_INV','REGISTER_CONFIG_SYSTEM_IPS','REGISTER_CONFIG_SYSTEM_LCS','REGISTER_CONFIG_SYSTEM_LEAD_UL','REGISTER_CONFIG_SYSTEM_LQ','REGISTER_CONFIG_SYSTEM_MMS','REGISTER_CONFIG_SYSTEM_MRP','REGISTER_CONFIG_SYSTEM_MUREX','REGISTER_CONFIG_SYSTEM_OBM','REGISTER_CONFIG_SYSTEM_OLS','REGISTER_CONFIG_SYSTEM_PDPA','REGISTER_CONFIG_SYSTEM_PLPS','REGISTER_CONFIG_SYSTEM_PMH','REGISTER_CONFIG_SYSTEM_PRM','REGISTER_CONFIG_SYSTEM_RBF','REGISTER_CONFIG_SYSTEM_RCR','REGISTER_CONFIG_SYSTEM_RDS','REGISTER_CONFIG_SYSTEM_SBG','REGISTER_CONFIG_SYSTEM_TMS','REGISTER_CONFIG_SYSTEM_TRD','REGISTER_CONFIG_SYSTEM_WLS','REGISTER_CONFIG_SYSTEM_WSS','REGISTER_CONFIG_SYSTEM_SCBL']</t>
+          <t>MVP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>['INT_L_BI_EDW_PARAM_ATS_COMP_CD']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>- LIST_SCHEMA_NAME</t>
+          <t>MVP6</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>['DSGEDW','FILE','FILE','FILE','FILE','FILE','FILE','FILE','FILE','FILE','FILE','FILE','FILE','VEULQ','VEULQ','VEULQ','VEULQ','VEULQ','VEULQ','VEULQ','VEULQ','VEURCR']</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>- LIST_TABLE_NAME</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>['RBF_SDL_CLEANSING_1_0','CCP_TXNALSB2K_1_0','VLQ_01_IM_ST_DAILY','VLQ_03_GL_RC_SEGMENT','VLQ_04_GL_OC_SEGMENT','VLQ_05_GL_ACCT_SEGMENT','VLQ_06_GL_PROD_SEGMENT','VLQ_07_GL_BAL_SUM_RC_D','VLQ_08_GL_BAL_SUM_OC_D','VLQ_09_LN_BR_FOREIGN_MKT_D','VRCR_FES_RCNCL_PNTX_TIMEOUT','WLS_WLSPARAM_1_0','WLS_WLSPROD_1_0','VLQ_01_IM_ST_DAILY','VLQ_03_GL_RC_SEGMENT','VLQ_04_GL_OC_SEGMENT','VLQ_05_GL_ACCT_SEGMENT','VLQ_06_GL_PROD_SEGMENT','VLQ_07_GL_BAL_SUM_RC_D','VLQ_08_GL_BAL_SUM_OC_D','VLQ_09_LN_BR_FOREIGN_MKT_D','VRCR_FES_RCNCL_PNTX_TIMEOUT']</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>- LIST DDL</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
           <t>[]</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>MVP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ATM,GN,INV,LCS,MMS,MUREX,PLPS,PMH</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>MVP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ATM,BCM,CCP,CFO,CHYO,EFS,IPS,LQ,PDPA,PMH,RCR,TMS,WLS</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MVP3</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ACTM,AM,BCC,CB,CCB,CIM,CSENT,CVA,ESN,FES,LEAD_UL,MRP,OLS,PRM,RBF,TRD,WSS</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>MVP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>BI,BIFI,EDW,ESL,SBG</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>MVP6</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>AML,CDD,CSM,ENL,LCS,OBM,RDS,SCBL</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>MVP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>['REGISTER_CONFIG_SYSTEM_ATM','REGISTER_CONFIG_SYSTEM_GN','REGISTER_CONFIG_SYSTEM_INV','REGISTER_CONFIG_SYSTEM_LCS','REGISTER_CONFIG_SYSTEM_MMS','REGISTER_CONFIG_SYSTEM_MUREX','REGISTER_CONFIG_SYSTEM_PLPS','REGISTER_CONFIG_SYSTEM_PMH']</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>MVP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>['REGISTER_CONFIG_SYSTEM_ATM','REGISTER_CONFIG_SYSTEM_BCM','REGISTER_CONFIG_SYSTEM_CCP','REGISTER_CONFIG_SYSTEM_CFO','REGISTER_CONFIG_SYSTEM_CHYO','REGISTER_CONFIG_SYSTEM_EFS','REGISTER_CONFIG_SYSTEM_IPS','REGISTER_CONFIG_SYSTEM_LQ','REGISTER_CONFIG_SYSTEM_PDPA','REGISTER_CONFIG_SYSTEM_PMH','REGISTER_CONFIG_SYSTEM_RCR','REGISTER_CONFIG_SYSTEM_TMS','REGISTER_CONFIG_SYSTEM_WLS']</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MVP3</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>['REGISTER_CONFIG_SYSTEM_ACTM','REGISTER_CONFIG_SYSTEM_AM','REGISTER_CONFIG_SYSTEM_BCC','REGISTER_CONFIG_SYSTEM_CB','REGISTER_CONFIG_SYSTEM_CCB','REGISTER_CONFIG_SYSTEM_CIM','REGISTER_CONFIG_SYSTEM_CSENT','REGISTER_CONFIG_SYSTEM_CVA','REGISTER_CONFIG_SYSTEM_ESN','REGISTER_CONFIG_SYSTEM_FES','REGISTER_CONFIG_SYSTEM_LEAD_UL','REGISTER_CONFIG_SYSTEM_MRP','REGISTER_CONFIG_SYSTEM_OLS','REGISTER_CONFIG_SYSTEM_PRM','REGISTER_CONFIG_SYSTEM_RBF','REGISTER_CONFIG_SYSTEM_TRD','REGISTER_CONFIG_SYSTEM_WSS']</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>MVP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>['REGISTER_CONFIG_SYSTEM_BI','REGISTER_CONFIG_SYSTEM_BIFI','REGISTER_CONFIG_SYSTEM_EDW','REGISTER_CONFIG_SYSTEM_ESL','REGISTER_CONFIG_SYSTEM_SBG']</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>MVP6</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>['REGISTER_CONFIG_SYSTEM_AML','REGISTER_CONFIG_SYSTEM_CDD','REGISTER_CONFIG_SYSTEM_CSM','REGISTER_CONFIG_SYSTEM_ENL','REGISTER_CONFIG_SYSTEM_LCS','REGISTER_CONFIG_SYSTEM_OBM','REGISTER_CONFIG_SYSTEM_RDS','REGISTER_CONFIG_SYSTEM_SCBL']</t>
         </is>
       </c>
     </row>

</xml_diff>